<commit_message>
changed some names and professions
</commit_message>
<xml_diff>
--- a/Encoding_Recall/Profession_condition.xlsx
+++ b/Encoding_Recall/Profession_condition.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hassl\OneDrive - Lund University\Biofinder\fMRI-tasks\FacesNamesProfessions_fMRI\Encoding_Recall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71371EF4-3E25-4925-98F9-F060AFAB9789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC28D0DD-23F1-40C3-9C63-0AE01B3016E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="11890" windowWidth="19420" windowHeight="10420" xr2:uid="{35F75019-C1EC-4D94-B52C-EFFB06201ACB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{35F75019-C1EC-4D94-B52C-EFFB06201ACB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Images_Faces/SH31.png</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>Proffession</t>
-  </si>
-  <si>
-    <t>order_randomiser</t>
   </si>
   <si>
     <t>Bagare</t>
@@ -251,12 +248,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,10 +280,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,13 +604,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BC7F93-5BEE-4667-9EAB-305B6EB07A60}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -607,401 +620,295 @@
       <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D31" ca="1" si="0">RAND()</f>
-        <v>0.24734276736148963</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45478445938417233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7433803586737442E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32402551859466056</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32172730747814826</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.22605714690624035</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.67328253538770344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.27664949845648457</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.26857216169068832</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.66612128584873787</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.2097558878752076</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43173067737053561</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5506161487107066E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.58618414217940507</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    </row>
+    <row r="27" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.38502199212498567</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.90922163476461282</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.82123048642722263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.98546065839881913</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49847430071286436</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.71677711559731172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.10881627067326916</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.1223308811919066</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.73086705093862359</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.28218757218131041</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3749649037832139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.16067568711583546</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1009,64 +916,48 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32253446998245239</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.78185489531122199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43651711907022228</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.94521093736733464</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
-    <sortCondition ref="D2:D31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
+    <sortCondition ref="A2:A33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>